<commit_message>
clean and update qdrant
</commit_message>
<xml_diff>
--- a/data/locais_com_quintas_destacadas_ATUALIZADO_v2.xlsx
+++ b/data/locais_com_quintas_destacadas_ATUALIZADO_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euroconsumers-my.sharepoint.com/personal/mib_portugal_conseur_org/Documents/Documents/Personal/Viagens/PassagemAno/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euroconsumers-my.sharepoint.com/personal/mib_portugal_conseur_org/Documents/Documents/Personal/PROJECTOS/CHATBOT AI/chatbot/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="418" documentId="8_{39105DAE-58B3-4AFD-93ED-5BC3F167168E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CD18E6B-B460-413A-AE17-1A6F75330993}"/>
+  <xr:revisionPtr revIDLastSave="438" documentId="8_{39105DAE-58B3-4AFD-93ED-5BC3F167168E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D017785B-B047-4C24-9702-F8847DE5721B}"/>
   <bookViews>
-    <workbookView xWindow="744" yWindow="504" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="396" yWindow="156" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Locais" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="318">
   <si>
     <t>Nome</t>
   </si>
@@ -1018,9 +1018,6 @@
     <t>Website</t>
   </si>
   <si>
-    <t>Pousada de Juventude de Viana</t>
-  </si>
-  <si>
     <t>bgdocampo@gmail.com</t>
   </si>
   <si>
@@ -1048,12 +1045,6 @@
     <t>Erro email</t>
   </si>
   <si>
-    <t>Pousada de Valença (Pestana)</t>
-  </si>
-  <si>
-    <t>WOT (WOT Peniche)</t>
-  </si>
-  <si>
     <t>Zona</t>
   </si>
   <si>
@@ -1067,6 +1058,9 @@
   </si>
   <si>
     <t>Pontevedra</t>
+  </si>
+  <si>
+    <t>para esas fechas ya tenemos todas las casas ocupadas.</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1070,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1097,12 +1091,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9.6"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1161,49 +1149,10 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1213,7 +1162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1249,15 +1198,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1290,20 +1230,20 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCCC"/>
       <color rgb="FFFFFFCC"/>
       <color rgb="FFFFFF99"/>
-      <color rgb="FFFFCCCC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1317,6 +1257,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{87EF6CE9-CC8C-4221-80DE-BF827DD5EC01}" name="Table1" displayName="Table1" ref="A1:U36" totalsRowShown="0">
   <autoFilter ref="A1:U36" xr:uid="{87EF6CE9-CC8C-4221-80DE-BF827DD5EC01}"/>
@@ -1325,13 +1269,13 @@
     <tableColumn id="21" xr3:uid="{5FF2721C-AD90-42B0-BEEC-72423847E1A3}" name="Zona"/>
     <tableColumn id="5" xr3:uid="{F98FB781-034D-4E32-BEBB-ACBA0593BF71}" name="Morada"/>
     <tableColumn id="2" xr3:uid="{93D71D66-25E5-4CD9-AF59-6D09C83143C1}" name="Email"/>
-    <tableColumn id="3" xr3:uid="{23511D58-AE04-4A10-A09C-9C36322BF955}" name="Telefone" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{23511D58-AE04-4A10-A09C-9C36322BF955}" name="Telefone" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{886A49DD-921E-4B57-9A87-A146B3B75A2C}" name="Website"/>
     <tableColumn id="13" xr3:uid="{905C814F-F75F-4071-8D0F-A000269BD0DE}" name="Estado"/>
     <tableColumn id="14" xr3:uid="{D05F02CE-886C-4590-BBE6-4E9E2BBF1A12}" name="Resposta"/>
     <tableColumn id="15" xr3:uid="{994B9915-33EC-49EC-BFA8-FB170271383A}" name="Capacidade ≥ 43?"/>
     <tableColumn id="16" xr3:uid="{A93378A9-41CD-412D-8D73-DDA171FBADF6}" name="≤ 4 500 € (5 noites)?"/>
-    <tableColumn id="12" xr3:uid="{E8E69579-9C61-4F80-8BCD-9F9BC50334A9}" name="Estimativa custo (5 noites)" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{E8E69579-9C61-4F80-8BCD-9F9BC50334A9}" name="Estimativa custo (5 noites)" dataDxfId="0"/>
     <tableColumn id="7" xr3:uid="{99313F93-380B-4255-825E-22298F00107C}" name="Capacidade (n.º pessoas, confirmada)"/>
     <tableColumn id="9" xr3:uid="{F608F963-F4FF-40BE-BFBB-F739BB9147D8}" name="Última resposta (data)"/>
     <tableColumn id="11" xr3:uid="{9DFC6D75-0AA1-4738-9864-9FD05379F1A3}" name="Proposta tarifária (detalhe)"/>
@@ -1632,10 +1576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF70"/>
+  <dimension ref="A1:AD36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30:H36"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1673,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C1" t="s">
         <v>224</v>
@@ -1734,51 +1678,57 @@
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="H2" t="s">
-        <v>218</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="3" t="s">
+      <c r="H2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="15"/>
+      <c r="L2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3" t="s">
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="4">
         <v>3</v>
       </c>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3" t="s">
+      <c r="Q2" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="4" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1795,7 +1745,7 @@
       <c r="D3" t="s">
         <v>163</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="20" t="s">
         <v>164</v>
       </c>
       <c r="F3" t="s">
@@ -1822,7 +1772,7 @@
       <c r="D4" t="s">
         <v>146</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="20" t="s">
         <v>206</v>
       </c>
       <c r="F4" t="s">
@@ -1858,7 +1808,7 @@
       <c r="D5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="21" t="s">
         <v>42</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -1921,7 +1871,7 @@
       <c r="D6" t="s">
         <v>212</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="20" t="s">
         <v>213</v>
       </c>
       <c r="F6" t="s">
@@ -1948,7 +1898,7 @@
       <c r="D7" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="22" t="s">
         <v>93</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -1997,7 +1947,7 @@
       <c r="D8" t="s">
         <v>208</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="20" t="s">
         <v>209</v>
       </c>
       <c r="F8" t="s">
@@ -2024,7 +1974,7 @@
       <c r="D9" t="s">
         <v>150</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="20" t="s">
         <v>151</v>
       </c>
       <c r="F9" t="s">
@@ -2034,7 +1984,7 @@
         <v>220</v>
       </c>
       <c r="H9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K9" s="10"/>
       <c r="O9" t="s">
@@ -2060,7 +2010,7 @@
       <c r="D10" t="s">
         <v>183</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="20" t="s">
         <v>184</v>
       </c>
       <c r="F10" t="s">
@@ -2087,7 +2037,7 @@
       <c r="D11" t="s">
         <v>167</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="20" t="s">
         <v>168</v>
       </c>
       <c r="F11" t="s">
@@ -2112,7 +2062,7 @@
         <v>64</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="25"/>
+      <c r="E12" s="22"/>
       <c r="F12" s="5" t="s">
         <v>63</v>
       </c>
@@ -2170,7 +2120,7 @@
       <c r="D13" t="s">
         <v>171</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="20" t="s">
         <v>172</v>
       </c>
       <c r="F13" t="s">
@@ -2206,7 +2156,7 @@
       <c r="D14" t="s">
         <v>179</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="20" t="s">
         <v>180</v>
       </c>
       <c r="F14" t="s">
@@ -2242,7 +2192,7 @@
       <c r="D15" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="22" t="s">
         <v>81</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -2305,7 +2255,7 @@
       <c r="D16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="23" t="s">
         <v>17</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -2350,7 +2300,7 @@
       <c r="D17" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="22" t="s">
         <v>100</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -2395,7 +2345,7 @@
         <v>71</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="27"/>
+      <c r="E18" s="24"/>
       <c r="F18" s="2" t="s">
         <v>70</v>
       </c>
@@ -2458,7 +2408,7 @@
       <c r="D19" t="s">
         <v>187</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="20" t="s">
         <v>188</v>
       </c>
       <c r="F19" t="s">
@@ -2485,7 +2435,7 @@
       <c r="D20" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="25" t="s">
         <v>192</v>
       </c>
       <c r="F20" s="3" t="s">
@@ -2513,7 +2463,7 @@
         <v>53</v>
       </c>
       <c r="D21" s="5"/>
-      <c r="E21" s="25"/>
+      <c r="E21" s="22"/>
       <c r="F21" s="5" t="s">
         <v>52</v>
       </c>
@@ -2576,7 +2526,7 @@
       <c r="D22" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="25" t="s">
         <v>202</v>
       </c>
       <c r="F22" s="3" t="s">
@@ -2606,7 +2556,7 @@
       <c r="D23" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="25" t="s">
         <v>197</v>
       </c>
       <c r="F23" s="3" t="s">
@@ -2636,7 +2586,7 @@
       <c r="D24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="24" t="s">
         <v>26</v>
       </c>
       <c r="F24" s="2" t="s">
@@ -2699,7 +2649,7 @@
       <c r="D25" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="E25" s="26" t="s">
         <v>158</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -2744,7 +2694,7 @@
       <c r="D26" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="E26" s="27" t="s">
         <v>105</v>
       </c>
       <c r="F26" s="16" t="s">
@@ -2803,7 +2753,7 @@
       <c r="D27" t="s">
         <v>175</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="20" t="s">
         <v>176</v>
       </c>
       <c r="F27" t="s">
@@ -2830,7 +2780,7 @@
       <c r="D28" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="E28" s="23"/>
+      <c r="E28" s="20"/>
       <c r="F28" t="s">
         <v>276</v>
       </c>
@@ -2844,15 +2794,15 @@
         <v>277</v>
       </c>
       <c r="B29" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C29" t="s">
         <v>278</v>
       </c>
-      <c r="D29" s="22" t="s">
-        <v>304</v>
-      </c>
-      <c r="E29" s="23">
+      <c r="D29" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="E29" s="20">
         <v>34607722065</v>
       </c>
       <c r="F29" t="s">
@@ -2868,15 +2818,15 @@
         <v>280</v>
       </c>
       <c r="B30" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C30" t="s">
         <v>281</v>
       </c>
       <c r="D30" t="s">
-        <v>305</v>
-      </c>
-      <c r="E30" s="23">
+        <v>304</v>
+      </c>
+      <c r="E30" s="20">
         <v>34982505002</v>
       </c>
       <c r="F30" t="s">
@@ -2886,7 +2836,7 @@
         <v>220</v>
       </c>
       <c r="H30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K30" s="10"/>
     </row>
@@ -2895,15 +2845,15 @@
         <v>283</v>
       </c>
       <c r="B31" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C31" t="s">
         <v>284</v>
       </c>
       <c r="D31" t="s">
-        <v>306</v>
-      </c>
-      <c r="E31" s="23">
+        <v>305</v>
+      </c>
+      <c r="E31" s="20">
         <v>34981748156</v>
       </c>
       <c r="F31" t="s">
@@ -2919,15 +2869,15 @@
         <v>286</v>
       </c>
       <c r="B32" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C32" t="s">
         <v>287</v>
       </c>
       <c r="D32" t="s">
-        <v>307</v>
-      </c>
-      <c r="E32" s="23">
+        <v>306</v>
+      </c>
+      <c r="E32" s="20">
         <v>34981428149</v>
       </c>
       <c r="F32" t="s">
@@ -2943,15 +2893,15 @@
         <v>289</v>
       </c>
       <c r="B33" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C33" t="s">
         <v>290</v>
       </c>
       <c r="D33" t="s">
-        <v>308</v>
-      </c>
-      <c r="E33" s="23">
+        <v>307</v>
+      </c>
+      <c r="E33" s="20">
         <v>34981886432</v>
       </c>
       <c r="F33" t="s">
@@ -2967,15 +2917,15 @@
         <v>292</v>
       </c>
       <c r="B34" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C34" t="s">
         <v>293</v>
       </c>
       <c r="D34" t="s">
-        <v>309</v>
-      </c>
-      <c r="E34" s="23">
+        <v>308</v>
+      </c>
+      <c r="E34" s="20">
         <v>34986582122</v>
       </c>
       <c r="F34" t="s">
@@ -2991,15 +2941,15 @@
         <v>295</v>
       </c>
       <c r="B35" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C35" t="s">
         <v>296</v>
       </c>
-      <c r="D35" s="22" t="s">
-        <v>310</v>
-      </c>
-      <c r="E35" s="23">
+      <c r="D35" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="E35" s="20">
         <v>34986771242</v>
       </c>
       <c r="F35" t="s">
@@ -3009,7 +2959,7 @@
         <v>220</v>
       </c>
       <c r="H35" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K35" s="10"/>
     </row>
@@ -3018,15 +2968,15 @@
         <v>298</v>
       </c>
       <c r="B36" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C36" t="s">
         <v>299</v>
       </c>
       <c r="D36" t="s">
-        <v>311</v>
-      </c>
-      <c r="E36" s="23">
+        <v>310</v>
+      </c>
+      <c r="E36" s="20">
         <v>34981418146</v>
       </c>
       <c r="F36" t="s">
@@ -3036,140 +2986,9 @@
         <v>220</v>
       </c>
       <c r="H36" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K36" s="10"/>
-    </row>
-    <row r="44" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D45" s="19" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D46" s="20" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D47" s="20" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D48" s="20" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D49" s="20" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D50" s="20" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="51" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D51" s="20" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="52" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D52" s="20" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="53" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D53" s="20" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="54" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D54" s="20" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="55" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D55" s="20" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="56" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D56" s="20" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="57" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D57" s="20" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="58" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D58" s="20" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="59" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D59" s="20" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="60" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D60" s="20" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="61" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D61" s="20" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="62" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D62" s="20" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="63" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D63" s="20" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="64" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D64" s="20" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="65" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D65" s="20" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="66" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D66" s="20" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="67" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D67" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="68" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D68" s="20" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="69" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D69" s="20" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D70" s="21" t="s">
-        <v>314</v>
-      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U27">

</xml_diff>